<commit_message>
added controller method for downloading ServiceReport
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/serviceReport.xlsx
+++ b/src/main/resources/templates/serviceReport.xlsx
@@ -843,7 +843,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -917,6 +917,225 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -935,9 +1154,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -947,221 +1163,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1470,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22:L35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1489,51 +1501,51 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31" t="s">
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32" t="s">
+      <c r="I2" s="104"/>
+      <c r="J2" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
       <c r="J3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1543,392 +1555,392 @@
     <row r="4" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="108"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="20.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33" t="s">
+      <c r="B5" s="97"/>
+      <c r="C5" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33" t="s">
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="33"/>
+      <c r="H5" s="97"/>
       <c r="I5" s="23" t="s">
         <v>38</v>
       </c>
       <c r="J5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="97"/>
     </row>
     <row r="6" spans="1:12" ht="20.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
+      <c r="B6" s="98"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
       <c r="G6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="97"/>
       <c r="J6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
     </row>
     <row r="7" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33" t="s">
+      <c r="B7" s="97"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="97"/>
     </row>
     <row r="8" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="97"/>
       <c r="J8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
     </row>
     <row r="9" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="98"/>
+      <c r="H9" s="98"/>
+      <c r="I9" s="98"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="98"/>
+      <c r="L9" s="98"/>
     </row>
     <row r="10" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33" t="s">
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33" t="s">
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
+      <c r="K10" s="97"/>
+      <c r="L10" s="97"/>
     </row>
     <row r="11" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="99"/>
+      <c r="K11" s="99"/>
+      <c r="L11" s="99"/>
     </row>
     <row r="12" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="100"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="100"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="100"/>
+      <c r="L12" s="100"/>
     </row>
     <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="55" t="s">
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="56"/>
-      <c r="J13" s="53" t="s">
+      <c r="I13" s="92"/>
+      <c r="J13" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="55" t="s">
+      <c r="K13" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="L13" s="59"/>
+      <c r="L13" s="95"/>
     </row>
     <row r="14" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="60"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="93"/>
+      <c r="L14" s="96"/>
     </row>
     <row r="15" spans="1:12" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
+      <c r="A15" s="109"/>
+      <c r="B15" s="110"/>
+      <c r="C15" s="111"/>
+      <c r="D15" s="111"/>
+      <c r="E15" s="111"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="52"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="67"/>
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="52"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="67"/>
     </row>
     <row r="17" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="52"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="67"/>
     </row>
     <row r="18" spans="1:12" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="61"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="52"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="67"/>
     </row>
     <row r="19" spans="1:12" s="3" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="77"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
       <c r="J19" s="22"/>
-      <c r="K19" s="70"/>
-      <c r="L19" s="71"/>
+      <c r="K19" s="77"/>
+      <c r="L19" s="78"/>
     </row>
     <row r="20" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="81"/>
-      <c r="H20" s="81"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="61"/>
     </row>
     <row r="21" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="78" t="s">
+      <c r="B21" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="79"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="80"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="60"/>
       <c r="J21" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="67" t="s">
+      <c r="K21" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="L21" s="68"/>
+      <c r="L21" s="71"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
-      <c r="B22" s="82"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="84"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="64"/>
       <c r="J22" s="17"/>
-      <c r="K22" s="103"/>
-      <c r="L22" s="104"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="89"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="66"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="31"/>
       <c r="J23" s="18"/>
-      <c r="K23" s="105"/>
-      <c r="L23" s="106"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="36"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="66"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="31"/>
       <c r="J24" s="18"/>
-      <c r="K24" s="105"/>
-      <c r="L24" s="106"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="36"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="66"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="31"/>
       <c r="J25" s="18"/>
-      <c r="K25" s="105"/>
-      <c r="L25" s="106"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="36"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="66"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="31"/>
       <c r="J26" s="18"/>
-      <c r="K26" s="107"/>
-      <c r="L26" s="108"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="50"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
-      <c r="B27" s="64"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="66"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="31"/>
       <c r="J27" s="18"/>
-      <c r="K27" s="105"/>
-      <c r="L27" s="106"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="36"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
@@ -1941,50 +1953,50 @@
       <c r="H28" s="25"/>
       <c r="I28" s="26"/>
       <c r="J28" s="18"/>
-      <c r="K28" s="105"/>
-      <c r="L28" s="106"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="36"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="66"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="31"/>
       <c r="J29" s="18"/>
-      <c r="K29" s="105"/>
-      <c r="L29" s="106"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="36"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="66"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="31"/>
       <c r="J30" s="18"/>
-      <c r="K30" s="107"/>
-      <c r="L30" s="108"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="50"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="66"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="31"/>
       <c r="J31" s="18"/>
-      <c r="K31" s="105"/>
-      <c r="L31" s="106"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="36"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
@@ -1997,185 +2009,185 @@
       <c r="H32" s="25"/>
       <c r="I32" s="26"/>
       <c r="J32" s="18"/>
-      <c r="K32" s="105"/>
-      <c r="L32" s="106"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="36"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="66"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="31"/>
       <c r="J33" s="18"/>
-      <c r="K33" s="105"/>
-      <c r="L33" s="106"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="36"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
-      <c r="B34" s="64"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="66"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="31"/>
       <c r="J34" s="18"/>
-      <c r="K34" s="107"/>
-      <c r="L34" s="108"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="50"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
-      <c r="B35" s="64"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="66"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="31"/>
       <c r="J35" s="18"/>
-      <c r="K35" s="105"/>
-      <c r="L35" s="106"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="36"/>
     </row>
     <row r="36" spans="1:12" s="14" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="69" t="s">
+      <c r="A36" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="69"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="69"/>
-      <c r="J36" s="69"/>
-      <c r="K36" s="69"/>
-      <c r="L36" s="69"/>
+      <c r="B36" s="72"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="72"/>
     </row>
     <row r="37" spans="1:12" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="48"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="50"/>
+      <c r="A37" s="85"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="86"/>
+      <c r="H37" s="86"/>
+      <c r="I37" s="86"/>
+      <c r="J37" s="86"/>
+      <c r="K37" s="86"/>
+      <c r="L37" s="87"/>
     </row>
     <row r="38" spans="1:12" s="15" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="85" t="s">
+      <c r="A38" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="85"/>
-      <c r="C38" s="85"/>
-      <c r="D38" s="85"/>
-      <c r="E38" s="85"/>
-      <c r="F38" s="85"/>
-      <c r="G38" s="85"/>
-      <c r="H38" s="85"/>
-      <c r="I38" s="85"/>
-      <c r="J38" s="85"/>
-      <c r="K38" s="85"/>
-      <c r="L38" s="85"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
     </row>
     <row r="39" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="91" t="s">
+      <c r="B39" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="91"/>
-      <c r="D39" s="91"/>
-      <c r="E39" s="91"/>
-      <c r="F39" s="91"/>
-      <c r="G39" s="91"/>
-      <c r="H39" s="91"/>
-      <c r="I39" s="91"/>
-      <c r="J39" s="91"/>
-      <c r="K39" s="53" t="s">
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="L39" s="99"/>
+      <c r="L39" s="46"/>
     </row>
     <row r="40" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
-      <c r="B40" s="72"/>
-      <c r="C40" s="73"/>
-      <c r="D40" s="73"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="73"/>
-      <c r="I40" s="73"/>
-      <c r="J40" s="74"/>
-      <c r="K40" s="62"/>
-      <c r="L40" s="63"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="54"/>
+      <c r="K40" s="68"/>
+      <c r="L40" s="69"/>
     </row>
     <row r="41" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
-      <c r="B41" s="90"/>
-      <c r="C41" s="90"/>
-      <c r="D41" s="90"/>
-      <c r="E41" s="90"/>
-      <c r="F41" s="90"/>
-      <c r="G41" s="90"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="90"/>
-      <c r="J41" s="90"/>
-      <c r="K41" s="88"/>
-      <c r="L41" s="89"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="33"/>
     </row>
     <row r="42" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="102"/>
-      <c r="B42" s="102"/>
-      <c r="C42" s="102"/>
-      <c r="D42" s="102"/>
-      <c r="E42" s="102"/>
-      <c r="F42" s="102"/>
-      <c r="G42" s="102"/>
+      <c r="A42" s="51"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
     </row>
     <row r="43" spans="1:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="92" t="s">
+      <c r="A43" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="93"/>
-      <c r="C43" s="94"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="98"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
       <c r="G43" s="10"/>
-      <c r="H43" s="86" t="s">
+      <c r="H43" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="I43" s="86"/>
-      <c r="J43" s="100"/>
-      <c r="K43" s="100"/>
-      <c r="L43" s="100"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
     </row>
     <row r="44" spans="1:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="95"/>
-      <c r="B44" s="96"/>
-      <c r="C44" s="97"/>
-      <c r="D44" s="98"/>
-      <c r="E44" s="98"/>
-      <c r="F44" s="98"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
       <c r="G44" s="10"/>
-      <c r="H44" s="87"/>
-      <c r="I44" s="87"/>
-      <c r="J44" s="101"/>
-      <c r="K44" s="101"/>
-      <c r="L44" s="101"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="48"/>
+      <c r="K44" s="48"/>
+      <c r="L44" s="48"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
@@ -2188,6 +2200,86 @@
     </row>
   </sheetData>
   <mergeCells count="96">
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:L9"/>
+    <mergeCell ref="J10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="H10:I11"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="F10:G11"/>
+    <mergeCell ref="C10:E11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A37:L37"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="H13:I14"/>
+    <mergeCell ref="K13:L14"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B13:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="A36:L36"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="A38:L38"/>
+    <mergeCell ref="B24:I24"/>
     <mergeCell ref="H43:I44"/>
     <mergeCell ref="B33:I33"/>
     <mergeCell ref="B34:I34"/>
@@ -2204,86 +2296,6 @@
     <mergeCell ref="B35:I35"/>
     <mergeCell ref="K34:L34"/>
     <mergeCell ref="A42:G42"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="A36:L36"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A37:L37"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="H13:I14"/>
-    <mergeCell ref="K13:L14"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B13:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="J10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="H10:I11"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="F10:G11"/>
-    <mergeCell ref="C10:E11"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:J7"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.45" right="0.2" top="0.25" bottom="0" header="0.3" footer="0.3"/>

</xml_diff>